<commit_message>
rename fisch tabs ...
</commit_message>
<xml_diff>
--- a/tabs/Fisher_tests.xlsx
+++ b/tabs/Fisher_tests.xlsx
@@ -13,12 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
-  <si>
-    <t xml:space="preserve">var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+  <si>
+    <t xml:space="preserve">predictor</t>
   </si>
   <si>
     <t xml:space="preserve">p</t>
@@ -30,67 +27,103 @@
     <t xml:space="preserve">sig.</t>
   </si>
   <si>
-    <t xml:space="preserve">Antidepresiva.ano.ne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comb</t>
+    <t xml:space="preserve">Antidepressants * Diagnosis</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">marg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BDI.II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doba.žití.s.nemocí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS.míra.rizika.spavosti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F.1..M.2.</t>
+    <t xml:space="preserve">Antidepressants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDI-II * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDI-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease duration * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female1.Male2 * Diagnosis</t>
   </si>
   <si>
     <t xml:space="preserve">*</t>
   </si>
   <si>
-    <t xml:space="preserve">FSS.stupeň</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HADS.A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HADS.D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lék...který</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medikace.ano.ne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSS.stupeň</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psychiatrie..D.A.D.A..BAD.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frekvence.kataplexií</t>
-  </si>
-  <si>
-    <t xml:space="preserve">přítomnost.kataplexie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ve.vztahu..partnerství..manželství.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">věková.skupina</t>
+    <t xml:space="preserve">Female1.Male2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSS * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HADS-A * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HADS-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HADS-D * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HADS-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication narcolepsy (stimulants,sodium oxybate,pitolisant) * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication narcolepsy (stimulants,sodium oxybate,pitolisant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication narcolepsy (yes/no) * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication narcolepsy (yes/no)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSS * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychiatric disorder (depression, anxious-depressive disorder, bipolar disorder) * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychiatric disorder (depression, anxious-depressive disorder, bipolar disorder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosis (NT1,NT2, IH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cataplexy frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of cataplexy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single/in relationship * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single/in relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age * Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
   </si>
   <si>
     <t xml:space="preserve">issue</t>
@@ -570,535 +603,439 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.0845291547084529</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.556834431655683</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.573844261557384</v>
       </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="n">
+      <c r="B5" t="n">
         <v>0.808511914880851</v>
       </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.874331256687433</v>
       </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" t="n">
         <v>0.993010069899301</v>
       </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
       <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>0.0641493585064149</v>
       </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
       <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.268547314526855</v>
       </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" t="n">
         <v>0.025559744402556</v>
       </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="n">
+        <v>15</v>
+      </c>
+      <c r="B11" t="n">
         <v>0.0581894181058189</v>
       </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
       <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
+        <v>16</v>
+      </c>
+      <c r="B12" t="n">
         <v>0.0548294517054829</v>
       </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="n">
+        <v>17</v>
+      </c>
+      <c r="B13" t="n">
         <v>0.421485785142149</v>
       </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
+        <v>18</v>
+      </c>
+      <c r="B14" t="n">
         <v>0.0607493925060749</v>
       </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="n">
+        <v>19</v>
+      </c>
+      <c r="B15" t="n">
         <v>0.20209797902021</v>
       </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
+        <v>20</v>
+      </c>
+      <c r="B16" t="n">
         <v>0.158588414115859</v>
       </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
       <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="n">
+        <v>21</v>
+      </c>
+      <c r="B17" t="n">
         <v>0.82880171198288</v>
       </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
       <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
+        <v>22</v>
+      </c>
+      <c r="B18" t="n">
         <v>0.784642153578464</v>
       </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="n">
+        <v>23</v>
+      </c>
+      <c r="B19" t="n">
         <v>0.744472555274447</v>
       </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
       <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
+        <v>24</v>
+      </c>
+      <c r="B20" t="n">
         <v>0.0725192748072519</v>
       </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
       <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="n">
+        <v>25</v>
+      </c>
+      <c r="B21" t="n">
         <v>0.143148568514315</v>
       </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
       <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
+        <v>26</v>
+      </c>
+      <c r="B22" t="n">
         <v>0.867161328386716</v>
       </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
       <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="n">
+        <v>27</v>
+      </c>
+      <c r="B23" t="n">
         <v>0.818781812181878</v>
       </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
       <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n">
+        <v>28</v>
+      </c>
+      <c r="B24" t="n">
         <v>0.058269417305827</v>
       </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
       <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="n">
+        <v>29</v>
+      </c>
+      <c r="B25" t="n">
         <v>0.936210637893621</v>
       </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
       <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+      <c r="B26" t="n">
         <v>0.00602993970060299</v>
       </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
       <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="n">
+        <v>31</v>
+      </c>
+      <c r="B27" t="n">
         <v>0.887861121388786</v>
       </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
       <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="n">
+        <v>32</v>
+      </c>
+      <c r="B28" t="n">
         <v>0.453145468545315</v>
       </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
       <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" t="n">
+        <v>33</v>
+      </c>
+      <c r="B29" t="n">
         <v>0.309756902430976</v>
       </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
       <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="n">
+        <v>34</v>
+      </c>
+      <c r="B30" t="n">
         <v>0.558514414855851</v>
       </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
       <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="n">
+        <v>35</v>
+      </c>
+      <c r="B31" t="n">
         <v>0.332626673733263</v>
       </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
       <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="n">
+        <v>36</v>
+      </c>
+      <c r="B32" t="n">
         <v>0.542744572554274</v>
       </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
       <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1117,450 +1054,450 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>